<commit_message>
Update resources import template to include more resource divisions
</commit_message>
<xml_diff>
--- a/public/files/templates/resources.xlsx
+++ b/public/files/templates/resources.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omar.garana\Desktop\cost-control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/apps/cost-control/public/files/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="150001" calcMode="manual" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>RESOURCE
 CODE</t>
@@ -66,12 +72,20 @@
   <si>
     <t xml:space="preserve">RESOURCE
 TYPE </t>
+  </si>
+  <si>
+    <t>RESOURCE
+SUB DIVISION 3</t>
+  </si>
+  <si>
+    <t>RESOURCE
+SUB DIVISION 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -161,7 +175,26 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -181,9 +214,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -202,76 +232,22 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -293,29 +269,79 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,20 +357,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Resource" displayName="Resource" ref="A1:K2" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:K2"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="RESOURCE_x000a_TYPE " totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="23"/>
-    <tableColumn id="2" name="RESOURCE_x000a_DIVISION" dataDxfId="11" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="RESOURCE_x000a_SUB DIVISION 1" dataDxfId="10" totalsRowDxfId="21"/>
-    <tableColumn id="4" name="RESOURCE_x000a_SUB DIVISION 2" dataDxfId="9" totalsRowDxfId="20"/>
-    <tableColumn id="5" name="RESOURCE_x000a_CODE" dataDxfId="8" totalsRowDxfId="19"/>
-    <tableColumn id="6" name="RESOURCE_x000a_ NAME" dataDxfId="7" totalsRowDxfId="18"/>
-    <tableColumn id="7" name="STANDARD_x000a_RATE" dataDxfId="6" totalsRowDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="UNIT OF MEASURE" dataDxfId="5" totalsRowDxfId="16"/>
-    <tableColumn id="9" name="MATERIAL_x000a_Waste %" dataDxfId="4" totalsRowDxfId="15"/>
-    <tableColumn id="10" name="SUPPLIER/_x000a_SUBCON." dataDxfId="3" totalsRowDxfId="14"/>
-    <tableColumn id="11" name="REFERENCE" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Resource" displayName="Resource" ref="A1:M2" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:M2"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="RESOURCE_x000a_TYPE " totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="2" name="RESOURCE_x000a_DIVISION" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="3" name="RESOURCE_x000a_SUB DIVISION 1" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="4" name="RESOURCE_x000a_SUB DIVISION 2" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="12" name="RESOURCE_x000a_SUB DIVISION 3" dataDxfId="3" totalsRowDxfId="4"/>
+    <tableColumn id="13" name="RESOURCE_x000a_SUB DIVISION 4" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="RESOURCE_x000a_CODE" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="6" name="RESOURCE_x000a_ NAME" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="7" name="STANDARD_x000a_RATE" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="UNIT OF MEASURE" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="9" name="MATERIAL_x000a_Waste %" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="10" name="SUPPLIER/_x000a_SUBCON." dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="11" name="REFERENCE" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -613,28 +641,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -648,43 +676,51 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Refactor export resource to have the same template as import
</commit_message>
<xml_diff>
--- a/public/files/templates/resources.xlsx
+++ b/public/files/templates/resources.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Resources" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" calcMode="manual" concurrentCalc="0"/>
   <extLst>
@@ -156,19 +156,19 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -177,23 +177,7 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -211,7 +195,58 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -229,25 +264,16 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -269,61 +295,28 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -343,6 +336,13 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -357,22 +357,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Resource" displayName="Resource" ref="A1:M2" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Resource" displayName="Resource" ref="A1:M2" headerRowDxfId="27" dataDxfId="0">
   <autoFilter ref="A1:M2"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="RESOURCE_x000a_TYPE " totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="2" name="RESOURCE_x000a_DIVISION" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="3" name="RESOURCE_x000a_SUB DIVISION 1" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="4" name="RESOURCE_x000a_SUB DIVISION 2" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="12" name="RESOURCE_x000a_SUB DIVISION 3" dataDxfId="3" totalsRowDxfId="4"/>
-    <tableColumn id="13" name="RESOURCE_x000a_SUB DIVISION 4" dataDxfId="0" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="RESOURCE_x000a_CODE" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="6" name="RESOURCE_x000a_ NAME" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="7" name="STANDARD_x000a_RATE" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="UNIT OF MEASURE" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="9" name="MATERIAL_x000a_Waste %" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="10" name="SUPPLIER/_x000a_SUBCON." dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="11" name="REFERENCE" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" name="RESOURCE_x000a_TYPE " totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="26"/>
+    <tableColumn id="2" name="RESOURCE_x000a_DIVISION" dataDxfId="12" totalsRowDxfId="25"/>
+    <tableColumn id="3" name="RESOURCE_x000a_SUB DIVISION 1" dataDxfId="11" totalsRowDxfId="24"/>
+    <tableColumn id="4" name="RESOURCE_x000a_SUB DIVISION 2" dataDxfId="10" totalsRowDxfId="23"/>
+    <tableColumn id="12" name="RESOURCE_x000a_SUB DIVISION 3" dataDxfId="9" totalsRowDxfId="22"/>
+    <tableColumn id="13" name="RESOURCE_x000a_SUB DIVISION 4" dataDxfId="8" totalsRowDxfId="21"/>
+    <tableColumn id="5" name="RESOURCE_x000a_CODE" dataDxfId="7" totalsRowDxfId="20"/>
+    <tableColumn id="6" name="RESOURCE_x000a_ NAME" dataDxfId="6" totalsRowDxfId="19"/>
+    <tableColumn id="7" name="STANDARD_x000a_RATE" dataDxfId="5" totalsRowDxfId="18" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="UNIT OF MEASURE" dataDxfId="4" totalsRowDxfId="17"/>
+    <tableColumn id="9" name="MATERIAL_x000a_Waste %" dataDxfId="3" totalsRowDxfId="16"/>
+    <tableColumn id="10" name="SUPPLIER/_x000a_SUBCON." dataDxfId="2" totalsRowDxfId="15"/>
+    <tableColumn id="11" name="REFERENCE" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -720,7 +720,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>